<commit_message>
added scene functions and therefore had to rename ExcelDmxConnection to ExcelRuntime as it also manages the scenes
</commit_message>
<xml_diff>
--- a/doc/Excel/Test.xlsx
+++ b/doc/Excel/Test.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ccf072f8ee41ce39/Code/C^N und .NET/AuLiCom/AuLiComXL/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ccf072f8ee41ce39/Code/C^N und .NET/AuLiCom/doc/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="194" documentId="8_{A4C15E09-0D12-4FC3-91B3-BCC6B1FE6774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D935DE07-E7AF-4502-BB65-057FB6A72AF0}"/>
+  <xr:revisionPtr revIDLastSave="393" documentId="8_{A4C15E09-0D12-4FC3-91B3-BCC6B1FE6774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6AE8CF3-4DDB-4A51-903A-4EF93A5A238F}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="8565" windowWidth="28800" windowHeight="9435" xr2:uid="{AB2CF87F-81B4-4088-AE2E-2820582A8761}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{AB2CF87F-81B4-4088-AE2E-2820582A8761}"/>
   </bookViews>
   <sheets>
     <sheet name="Current Status" sheetId="1" r:id="rId1"/>
+    <sheet name="Scenes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>All Available Ports</t>
   </si>
@@ -119,6 +120,39 @@
   </si>
   <si>
     <t>COM6</t>
+  </si>
+  <si>
+    <t>Mixed</t>
+  </si>
+  <si>
+    <t>Select Scene with X --&gt;</t>
+  </si>
+  <si>
+    <t>Selected Scene</t>
+  </si>
+  <si>
+    <t>Fade Time</t>
+  </si>
+  <si>
+    <t>Scene Name --&gt;</t>
+  </si>
+  <si>
+    <t>Fade-in Seconds --&gt;</t>
+  </si>
+  <si>
+    <t>All Scenes</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Red Only</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -226,7 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
@@ -235,6 +269,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -556,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7476D4-702A-41D6-800C-4D12D2F7DEDB}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" activeCellId="2" sqref="F4 F8 F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,15 +656,15 @@
         <v>4</v>
       </c>
       <c r="E4" cm="1">
-        <f t="array" aca="1" ref="E4" ca="1">_xll.AuLiComGetChannelValue(D4)</f>
-        <v>50</v>
+        <f t="array" ref="E4">_xll.AuLiComGetChannelValue(D4)</f>
+        <v>0</v>
       </c>
       <c r="F4" s="2">
         <v>50</v>
       </c>
-      <c r="G4" s="3" t="str" cm="1">
-        <f t="array" aca="1" ref="G4" ca="1">IF(F4&lt;&gt;E4,_xll.AuLiComSetChannelValue(D4,F4),"")</f>
-        <v/>
+      <c r="G4" s="3" cm="1">
+        <f t="array" ref="G4">IF(F4&lt;&gt;E4,_xll.AuLiComSetChannelValue(D4,F4),"")</f>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -637,12 +680,12 @@
         <v>5</v>
       </c>
       <c r="E5" cm="1">
-        <f t="array" aca="1" ref="E5" ca="1">_xll.AuLiComGetChannelValue(D5)</f>
+        <f t="array" ref="E5">_xll.AuLiComGetChannelValue(D5)</f>
         <v>0</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="3" t="str" cm="1">
-        <f t="array" aca="1" ref="G5" ca="1">IF(F5&lt;&gt;E5,_xll.AuLiComSetChannelValue(D5,F5),"")</f>
+        <f t="array" ref="G5">IF(F5&lt;&gt;E5,_xll.AuLiComSetChannelValue(D5,F5),"")</f>
         <v/>
       </c>
     </row>
@@ -655,12 +698,12 @@
         <v>6</v>
       </c>
       <c r="E6" cm="1">
-        <f t="array" aca="1" ref="E6" ca="1">_xll.AuLiComGetChannelValue(D6)</f>
+        <f t="array" ref="E6">_xll.AuLiComGetChannelValue(D6)</f>
         <v>0</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="3" t="str" cm="1">
-        <f t="array" aca="1" ref="G6" ca="1">IF(F6&lt;&gt;E6,_xll.AuLiComSetChannelValue(D6,F6),"")</f>
+        <f t="array" ref="G6">IF(F6&lt;&gt;E6,_xll.AuLiComSetChannelValue(D6,F6),"")</f>
         <v/>
       </c>
     </row>
@@ -676,12 +719,12 @@
         <v>7</v>
       </c>
       <c r="E7" cm="1">
-        <f t="array" aca="1" ref="E7" ca="1">_xll.AuLiComGetChannelValue(D7)</f>
+        <f t="array" ref="E7">_xll.AuLiComGetChannelValue(D7)</f>
         <v>0</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="3" t="str" cm="1">
-        <f t="array" aca="1" ref="G7" ca="1">IF(F7&lt;&gt;E7,_xll.AuLiComSetChannelValue(D7,F7),"")</f>
+        <f t="array" ref="G7">IF(F7&lt;&gt;E7,_xll.AuLiComSetChannelValue(D7,F7),"")</f>
         <v/>
       </c>
     </row>
@@ -697,15 +740,15 @@
         <v>8</v>
       </c>
       <c r="E8" cm="1">
-        <f t="array" aca="1" ref="E8" ca="1">_xll.AuLiComGetChannelValue(D8)</f>
-        <v>50</v>
+        <f t="array" ref="E8">_xll.AuLiComGetChannelValue(D8)</f>
+        <v>0</v>
       </c>
       <c r="F8" s="2">
         <v>50</v>
       </c>
-      <c r="G8" s="3" t="str" cm="1">
-        <f t="array" aca="1" ref="G8" ca="1">IF(F8&lt;&gt;E8,_xll.AuLiComSetChannelValue(D8,F8),"")</f>
-        <v/>
+      <c r="G8" s="3" cm="1">
+        <f t="array" ref="G8">IF(F8&lt;&gt;E8,_xll.AuLiComSetChannelValue(D8,F8),"")</f>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -721,12 +764,12 @@
         <v>9</v>
       </c>
       <c r="E9" cm="1">
-        <f t="array" aca="1" ref="E9" ca="1">_xll.AuLiComGetChannelValue(D9)</f>
+        <f t="array" ref="E9">_xll.AuLiComGetChannelValue(D9)</f>
         <v>0</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="3" t="str" cm="1">
-        <f t="array" aca="1" ref="G9" ca="1">IF(F9&lt;&gt;E9,_xll.AuLiComSetChannelValue(D9,F9),"")</f>
+        <f t="array" ref="G9">IF(F9&lt;&gt;E9,_xll.AuLiComSetChannelValue(D9,F9),"")</f>
         <v/>
       </c>
     </row>
@@ -739,12 +782,12 @@
         <v>10</v>
       </c>
       <c r="E10" cm="1">
-        <f t="array" aca="1" ref="E10" ca="1">_xll.AuLiComGetChannelValue(D10)</f>
+        <f t="array" ref="E10">_xll.AuLiComGetChannelValue(D10)</f>
         <v>0</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="3" t="str" cm="1">
-        <f t="array" aca="1" ref="G10" ca="1">IF(F10&lt;&gt;E10,_xll.AuLiComSetChannelValue(D10,F10),"")</f>
+        <f t="array" ref="G10">IF(F10&lt;&gt;E10,_xll.AuLiComSetChannelValue(D10,F10),"")</f>
         <v/>
       </c>
     </row>
@@ -760,12 +803,12 @@
         <v>11</v>
       </c>
       <c r="E11" cm="1">
-        <f t="array" aca="1" ref="E11" ca="1">_xll.AuLiComGetChannelValue(D11)</f>
+        <f t="array" ref="E11">_xll.AuLiComGetChannelValue(D11)</f>
         <v>0</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="3" t="str" cm="1">
-        <f t="array" aca="1" ref="G11" ca="1">IF(F11&lt;&gt;E11,_xll.AuLiComSetChannelValue(D11,F11),"")</f>
+        <f t="array" ref="G11">IF(F11&lt;&gt;E11,_xll.AuLiComSetChannelValue(D11,F11),"")</f>
         <v/>
       </c>
     </row>
@@ -782,15 +825,15 @@
         <v>12</v>
       </c>
       <c r="E12" cm="1">
-        <f t="array" aca="1" ref="E12" ca="1">_xll.AuLiComGetChannelValue(D12)</f>
-        <v>50</v>
+        <f t="array" ref="E12">_xll.AuLiComGetChannelValue(D12)</f>
+        <v>0</v>
       </c>
       <c r="F12" s="2">
         <v>50</v>
       </c>
-      <c r="G12" s="3" t="str" cm="1">
-        <f t="array" aca="1" ref="G12" ca="1">IF(F12&lt;&gt;E12,_xll.AuLiComSetChannelValue(D12,F12),"")</f>
-        <v/>
+      <c r="G12" s="3" cm="1">
+        <f t="array" ref="G12">IF(F12&lt;&gt;E12,_xll.AuLiComSetChannelValue(D12,F12),"")</f>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -820,4 +863,357 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70329325-0127-4D2B-9411-22A514396505}">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="D2">
+        <v>0.25</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="str" cm="1">
+        <f t="array" ref="C5">_xll.AuLiComCreateScene(C1,$B$6:$B$14,C6:C14)</f>
+        <v>Mixed</v>
+      </c>
+      <c r="D5" s="3" t="str" cm="1">
+        <f t="array" ref="D5">_xll.AuLiComCreateScene(D1,$B$6:$B$14,D6:D14)</f>
+        <v>Red Only</v>
+      </c>
+      <c r="E5" s="3" t="str" cm="1">
+        <f t="array" ref="E5">_xll.AuLiComCreateScene(E1,$B$6:$B$14,E6:E14)</f>
+        <v>Black</v>
+      </c>
+      <c r="F5" s="3" t="str" cm="1">
+        <f t="array" ref="F5">_xll.AuLiComCreateScene(F1,$B$6:$B$14,F6:F14)</f>
+        <v>All</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <f>B6+1</f>
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ref="B8:B14" si="0">B7+1</f>
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>100</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="str" cm="1">
+        <f t="array" ref="B18">INDEX(1:1,1,_xlfn.XMATCH("X",15:15))</f>
+        <v>Mixed</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" cm="1">
+        <f t="array" ref="B19">INDEX(2:2,1,_xlfn.XMATCH("X",15:15))</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="str" cm="1">
+        <f t="array" ref="B20">_xll.AuLiComSetSingleActiveScene(B18,B19)</f>
+        <v>Mixed</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="str" cm="1">
+        <f t="array" ref="A24:A28">_xll.AuLiComGetScenes()</f>
+        <v>Mixed</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <v>All Red</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <v>Black</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <v>Red Only</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <v>All</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>